<commit_message>
back form the dead
</commit_message>
<xml_diff>
--- a/SoftwareList.xlsx
+++ b/SoftwareList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacharles\Desktop\work\models\financial_models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4F4735-7810-49E3-BB3B-C047E6DA8329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF4BFF8F-F8CB-43C8-B22B-DA86CE74863D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2385" yWindow="240" windowWidth="18615" windowHeight="14430" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="750" windowWidth="19530" windowHeight="20850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="484">
   <si>
     <t>Software Stocks</t>
   </si>
@@ -1471,6 +1471,12 @@
   </si>
   <si>
     <t>Treasure Global Inc.</t>
+  </si>
+  <si>
+    <t>SoFi Technology</t>
+  </si>
+  <si>
+    <t>SOFI</t>
   </si>
 </sst>
 </file>
@@ -1805,10 +1811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C2:D244"/>
+  <dimension ref="C2:D245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="D246" sqref="D246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3749,6 +3755,14 @@
         <v>480</v>
       </c>
     </row>
+    <row r="245" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C245" t="s">
+        <v>482</v>
+      </c>
+      <c r="D245" t="s">
+        <v>483</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>